<commit_message>
Reajuste - (faltando a função de salvar)
</commit_message>
<xml_diff>
--- a/dados_dos_alunos.xlsx
+++ b/dados_dos_alunos.xlsx
@@ -549,7 +549,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I156"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
       <selection activeCell="D115" sqref="D115"/>
@@ -5452,6 +5452,68 @@
         <v>0</v>
       </c>
     </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Abbc</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>12312312311</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>17415</v>
+      </c>
+      <c r="D157" t="n">
+        <v>1</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Padrão</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>COMP359, COMP360, COMP361, COMP362, COMP363</t>
+        </is>
+      </c>
+      <c r="G157" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Daniel Barbosa</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>12318207444</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>10855</v>
+      </c>
+      <c r="D158" t="n">
+        <v>1</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Padrão</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>COMP359, COMP360, COMP361, COMP362, COMP363</t>
+        </is>
+      </c>
+      <c r="G158" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>